<commit_message>
Fixed logic on cell checks
Specifically, had the NaN logic backwards.
</commit_message>
<xml_diff>
--- a/spec/sheets/works001-minimal.xlsx
+++ b/spec/sheets/works001-minimal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcjadud/git/FAC/xlsx/spec/sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9539FCD3-8A2A-954A-B61F-009C365D9586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF52672B-539D-7A47-B8B0-D0B22B386076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="860" windowWidth="20520" windowHeight="14200" xr2:uid="{DA1A9B60-C8C2-C54B-A827-41A908274057}"/>
+    <workbookView xWindow="260" yWindow="860" windowWidth="20520" windowHeight="14200" activeTab="1" xr2:uid="{DA1A9B60-C8C2-C54B-A827-41A908274057}"/>
   </bookViews>
   <sheets>
     <sheet name="Data_Entry" sheetId="1" r:id="rId1"/>
@@ -33,12 +33,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>uid</t>
   </si>
   <si>
     <t>FINDINGS_TEXT_2019-2022</t>
+  </si>
+  <si>
+    <t>Do not edit this sheet.</t>
   </si>
 </sst>
 </file>
@@ -54,12 +57,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -74,8 +83,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,7 +402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC58C028-BA10-F84E-A24D-046B6CCF6569}">
   <dimension ref="D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -410,10 +420,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F977ADCB-58E0-4C42-A15E-8E54E06FA573}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -421,13 +431,18 @@
     <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>